<commit_message>
Updated feature definitions - more complete, and including antisense
</commit_message>
<xml_diff>
--- a/tabular/reference_feature_locations.xlsx
+++ b/tabular/reference_feature_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="560" windowWidth="21460" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="15220" yWindow="1180" windowWidth="27240" windowHeight="23420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="82">
   <si>
     <t>featureName</t>
   </si>
@@ -226,9 +226,6 @@
     <t>gp2</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>KJ831064</t>
   </si>
   <si>
@@ -260,6 +257,18 @@
   </si>
   <si>
     <t>REF_Po-Circo-41</t>
+  </si>
+  <si>
+    <t>Cap-rev</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>Cyclovirus</t>
+  </si>
+  <si>
+    <t>Circovirus</t>
   </si>
 </sst>
 </file>
@@ -272,6 +281,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,7 +333,7 @@
       <name val="Courier New"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,12 +350,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000090"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -368,7 +372,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -382,7 +404,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1927">
+  <cellStyleXfs count="2027">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2310,8 +2332,108 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2321,14 +2443,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2343,9 +2461,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1927">
+  <cellStyles count="2027">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3310,6 +3433,56 @@
     <cellStyle name="Followed Hyperlink" xfId="1922" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1924" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1932" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1934" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1936" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1938" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1958" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1960" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1962" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1964" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1966" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1968" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1970" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1972" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1974" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1976" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1998" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2026" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -4272,6 +4445,56 @@
     <cellStyle name="Hyperlink" xfId="1921" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1923" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1931" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1933" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1935" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1937" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1957" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1959" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1961" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1963" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1965" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1967" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1969" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1971" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1973" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1975" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1997" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2013" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2015" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2017" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2019" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2021" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2025" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4606,25 +4829,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1503"/>
+  <dimension ref="A1:H1502"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D38" sqref="C27:D38"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14" style="9" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -4632,1840 +4855,2122 @@
         <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1261</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1761</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1240</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1974</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1154</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1906</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1116</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1928</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1212</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1961</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="6">
+        <v>614</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1063</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1190</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1927</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1020</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1703</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C10" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1038</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1730</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="6">
+        <v>357</v>
+      </c>
+      <c r="G11" s="6">
+        <v>671</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1034</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1735</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1336</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1980</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1116</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1844</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1251</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1934</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1190</v>
+      </c>
+      <c r="G16" s="6">
+        <v>2020</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="6">
+        <v>968</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1723</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1055</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1711</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="6">
+        <v>648</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1400</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="6">
+        <v>48</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1007</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="6">
+        <v>108</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1007</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="6">
+        <v>550</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1026</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="6">
+        <v>32</v>
+      </c>
+      <c r="G23" s="6">
+        <v>948</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="6">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>912</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="6">
+        <v>48</v>
+      </c>
+      <c r="G25" s="6">
+        <v>926</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="6">
+        <v>29</v>
+      </c>
+      <c r="G26" s="6">
+        <v>904</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" s="6">
+        <v>100</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1017</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F28" s="6">
+        <v>36</v>
+      </c>
+      <c r="G28" s="6">
+        <v>929</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="6">
+        <v>2</v>
+      </c>
+      <c r="G29" s="6">
+        <v>10</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" s="6">
+        <v>55</v>
+      </c>
+      <c r="G30" s="6">
+        <v>993</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="6">
+        <v>51</v>
+      </c>
+      <c r="G31" s="6">
+        <v>995</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F32" s="6">
+        <v>216</v>
+      </c>
+      <c r="G32" s="6">
+        <v>1106</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="6">
+        <v>36</v>
+      </c>
+      <c r="G33" s="6">
+        <v>911</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="6">
+        <v>251</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1195</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F35" s="6">
+        <v>37</v>
+      </c>
+      <c r="G35" s="6">
+        <v>906</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F36" s="6">
+        <v>48</v>
+      </c>
+      <c r="G36" s="6">
+        <v>929</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F37" s="6">
+        <v>8</v>
+      </c>
+      <c r="G37" s="6">
+        <v>919</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="6">
+        <v>29</v>
+      </c>
+      <c r="G38" s="6">
+        <v>904</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="6">
+        <v>208</v>
+      </c>
+      <c r="G39" s="6">
+        <v>867</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F40" s="6">
+        <v>1005</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1703</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="6">
+        <v>183</v>
+      </c>
+      <c r="G41" s="6">
+        <v>875</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F42" s="6">
+        <v>1685</v>
+      </c>
+      <c r="G42" s="6">
+        <v>855</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="6">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <v>10</v>
-      </c>
-      <c r="G2" s="8" t="s">
+      <c r="B43" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F43" s="6">
+        <v>606</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1583</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="6">
-        <v>55</v>
-      </c>
-      <c r="F3" s="6">
-        <v>993</v>
-      </c>
-      <c r="G3" s="8" t="s">
+    <row r="44" spans="1:8">
+      <c r="A44" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F44" s="6">
+        <v>1741</v>
+      </c>
+      <c r="G44" s="6">
+        <v>2313</v>
+      </c>
+      <c r="H44" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    <row r="45" spans="1:8">
+      <c r="A45" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="6">
-        <v>1038</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1730</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="7">
-        <v>51</v>
-      </c>
-      <c r="F5" s="7">
-        <v>995</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="F45" s="6">
+        <v>2329</v>
+      </c>
+      <c r="G45" s="6">
+        <v>2329</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="15">
-        <v>357</v>
-      </c>
-      <c r="F6" s="15">
-        <v>671</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1034</v>
-      </c>
-      <c r="F7" s="15">
-        <v>1735</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="6">
-        <v>216</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1106</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="6">
-        <v>1336</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1980</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7">
-        <v>912</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1116</v>
-      </c>
-      <c r="F11" s="7">
-        <v>1928</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="6">
-        <v>36</v>
-      </c>
-      <c r="F12" s="6">
-        <v>929</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="6">
-        <v>1020</v>
-      </c>
-      <c r="F13" s="6">
-        <v>1703</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="7">
-        <v>8</v>
-      </c>
-      <c r="F14" s="7">
-        <v>919</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1055</v>
-      </c>
-      <c r="F15" s="7">
-        <v>1711</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="6">
-        <v>108</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1007</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="6">
-        <v>550</v>
-      </c>
-      <c r="F17" s="6">
-        <v>1026</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1240</v>
-      </c>
-      <c r="F18" s="6">
-        <v>1974</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="7">
-        <v>32</v>
-      </c>
-      <c r="F19" s="7">
-        <v>948</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="7">
-        <v>275</v>
-      </c>
-      <c r="F20" s="7">
-        <v>679</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="7">
-        <v>1154</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1906</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="6">
-        <v>37</v>
-      </c>
-      <c r="F22" s="6">
-        <v>906</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="6">
-        <v>1190</v>
-      </c>
-      <c r="F23" s="6">
-        <v>2020</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="7">
-        <v>36</v>
-      </c>
-      <c r="F24" s="7">
-        <v>911</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="7">
-        <v>1116</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1844</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" s="6">
-        <v>100</v>
-      </c>
-      <c r="F26" s="6">
-        <v>1017</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1190</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1927</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="7">
-        <v>29</v>
-      </c>
-      <c r="F28" s="7">
-        <v>904</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="7">
-        <v>614</v>
-      </c>
-      <c r="F29" s="7">
-        <v>1063</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="6">
-        <v>48</v>
-      </c>
-      <c r="F30" s="6">
-        <v>926</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="6">
-        <v>1212</v>
-      </c>
-      <c r="F31" s="6">
-        <v>1961</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="7">
-        <v>48</v>
-      </c>
-      <c r="F32" s="7">
-        <v>929</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E33" s="7">
-        <v>968</v>
-      </c>
-      <c r="F33" s="7">
-        <v>1723</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" s="6">
-        <v>29</v>
-      </c>
-      <c r="F34" s="6">
-        <v>904</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E35" s="6">
-        <v>648</v>
-      </c>
-      <c r="F35" s="6">
-        <v>1400</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" s="7">
-        <v>48</v>
-      </c>
-      <c r="F36" s="7">
-        <v>1007</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="7">
-        <v>1261</v>
-      </c>
-      <c r="F37" s="7">
-        <v>1761</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="6">
-        <v>251</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1195</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" s="6">
-        <v>1251</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1934</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B40" t="s">
-        <v>70</v>
-      </c>
-      <c r="C40" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40">
-        <v>183</v>
-      </c>
-      <c r="F40">
-        <v>875</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>70</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41">
-        <v>855</v>
-      </c>
-      <c r="F41">
-        <v>1685</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E42" s="6">
-        <v>208</v>
-      </c>
-      <c r="F42" s="6">
-        <v>867</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E43" s="6">
-        <v>1005</v>
-      </c>
-      <c r="F43" s="6">
-        <v>1703</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" t="s">
-        <v>77</v>
-      </c>
-      <c r="C44" t="s">
-        <v>78</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E44">
-        <v>606</v>
-      </c>
-      <c r="F44">
-        <v>1583</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" t="s">
-        <v>78</v>
-      </c>
-      <c r="D45"/>
-      <c r="E45">
-        <v>1741</v>
-      </c>
-      <c r="F45">
-        <v>2313</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" t="s">
-        <v>77</v>
-      </c>
-      <c r="C46" t="s">
-        <v>78</v>
-      </c>
-      <c r="D46"/>
-      <c r="E46">
-        <v>2329</v>
-      </c>
-      <c r="F46">
-        <v>2329</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4" ht="14" customHeight="1"/>
-    <row r="57" spans="4:4">
-      <c r="D57" s="12"/>
-    </row>
-    <row r="62" spans="4:4" ht="16" customHeight="1"/>
-    <row r="71" spans="2:6">
+    <row r="56" spans="5:5" ht="14" customHeight="1">
+      <c r="E56" s="10"/>
+    </row>
+    <row r="62" spans="5:5" ht="16" customHeight="1"/>
+    <row r="70" spans="2:7">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="11"/>
+    </row>
+    <row r="71" spans="2:7">
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
-      <c r="D71" s="13"/>
-    </row>
-    <row r="72" spans="2:6">
+      <c r="D71" s="2"/>
+      <c r="E71" s="11"/>
+    </row>
+    <row r="72" spans="2:7">
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="13"/>
-    </row>
-    <row r="73" spans="2:6">
+      <c r="D72" s="2"/>
+      <c r="E72" s="11"/>
+    </row>
+    <row r="73" spans="2:7">
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
-      <c r="D73" s="13"/>
-    </row>
-    <row r="74" spans="2:6">
+      <c r="D73" s="2"/>
+      <c r="E73" s="11"/>
+    </row>
+    <row r="74" spans="2:7">
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
-      <c r="D74" s="13"/>
-    </row>
-    <row r="75" spans="2:6">
+      <c r="D74" s="2"/>
+      <c r="E74" s="11"/>
+    </row>
+    <row r="75" spans="2:7">
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
-      <c r="D75" s="13"/>
-    </row>
-    <row r="76" spans="2:6">
+      <c r="D75" s="2"/>
+      <c r="E75" s="11"/>
+    </row>
+    <row r="76" spans="2:7">
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
-      <c r="D76" s="13"/>
-    </row>
-    <row r="77" spans="2:6">
+      <c r="D76" s="2"/>
+      <c r="E76" s="11"/>
+    </row>
+    <row r="77" spans="2:7">
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
-      <c r="D77" s="13"/>
-    </row>
-    <row r="78" spans="2:6">
+      <c r="D77" s="2"/>
+      <c r="E77" s="11"/>
+    </row>
+    <row r="78" spans="2:7">
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="13"/>
-    </row>
-    <row r="79" spans="2:6">
+      <c r="D78" s="2"/>
+      <c r="E78" s="11"/>
+    </row>
+    <row r="79" spans="2:7">
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
-      <c r="D79" s="13"/>
-    </row>
-    <row r="80" spans="2:6">
+      <c r="D79" s="2"/>
+      <c r="E79" s="11"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="2:7">
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
-      <c r="D80" s="13"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="2:6">
+      <c r="D80" s="2"/>
+      <c r="E80" s="11"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="2:5">
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
-      <c r="D81" s="13"/>
-      <c r="F81" s="2"/>
-    </row>
-    <row r="82" spans="2:6">
+      <c r="D81" s="2"/>
+      <c r="E81" s="11"/>
+    </row>
+    <row r="82" spans="2:5">
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
-      <c r="D82" s="13"/>
-    </row>
-    <row r="83" spans="2:6">
+      <c r="D82" s="2"/>
+      <c r="E82" s="11"/>
+    </row>
+    <row r="83" spans="2:5">
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
-      <c r="D83" s="13"/>
-    </row>
-    <row r="84" spans="2:6">
+      <c r="D83" s="2"/>
+      <c r="E83" s="11"/>
+    </row>
+    <row r="84" spans="2:5">
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="13"/>
-    </row>
-    <row r="85" spans="2:6">
+      <c r="D84" s="2"/>
+      <c r="E84" s="11"/>
+    </row>
+    <row r="85" spans="2:5">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
-      <c r="D85" s="13"/>
-    </row>
-    <row r="86" spans="2:6">
+      <c r="D85" s="2"/>
+      <c r="E85" s="11"/>
+    </row>
+    <row r="86" spans="2:5">
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
-      <c r="D86" s="13"/>
-    </row>
-    <row r="87" spans="2:6">
+      <c r="D86" s="2"/>
+      <c r="E86" s="11"/>
+    </row>
+    <row r="87" spans="2:5">
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
-      <c r="D87" s="13"/>
-    </row>
-    <row r="88" spans="2:6">
+      <c r="D87" s="2"/>
+      <c r="E87" s="11"/>
+    </row>
+    <row r="88" spans="2:5">
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
-      <c r="D88" s="13"/>
-    </row>
-    <row r="89" spans="2:6">
+      <c r="D88" s="2"/>
+      <c r="E88" s="11"/>
+    </row>
+    <row r="89" spans="2:5">
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
-      <c r="D89" s="13"/>
-    </row>
-    <row r="90" spans="2:6">
+      <c r="D89" s="2"/>
+      <c r="E89" s="11"/>
+    </row>
+    <row r="90" spans="2:5">
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
-      <c r="D90" s="13"/>
-    </row>
-    <row r="91" spans="2:6">
+      <c r="D90" s="2"/>
+      <c r="E90" s="11"/>
+    </row>
+    <row r="91" spans="2:5">
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
-      <c r="D91" s="13"/>
-    </row>
-    <row r="92" spans="2:6">
+      <c r="D91" s="2"/>
+      <c r="E91" s="11"/>
+    </row>
+    <row r="92" spans="2:5">
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
-      <c r="D92" s="13"/>
-    </row>
-    <row r="93" spans="2:6">
+      <c r="D92" s="2"/>
+      <c r="E92" s="11"/>
+    </row>
+    <row r="93" spans="2:5">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
-      <c r="D93" s="13"/>
-    </row>
-    <row r="94" spans="2:6">
+      <c r="D93" s="2"/>
+      <c r="E93" s="11"/>
+    </row>
+    <row r="94" spans="2:5">
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
-      <c r="D94" s="13"/>
-    </row>
-    <row r="95" spans="2:6">
+      <c r="D94" s="2"/>
+      <c r="E94" s="11"/>
+    </row>
+    <row r="95" spans="2:5">
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
-      <c r="D95" s="13"/>
-    </row>
-    <row r="96" spans="2:6">
+      <c r="D95" s="2"/>
+      <c r="E95" s="11"/>
+    </row>
+    <row r="96" spans="2:5">
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
-      <c r="D96" s="13"/>
-    </row>
-    <row r="97" spans="2:5">
+      <c r="D96" s="2"/>
+      <c r="E96" s="11"/>
+    </row>
+    <row r="97" spans="2:6">
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
-      <c r="D97" s="13"/>
-    </row>
-    <row r="98" spans="2:5">
+      <c r="D97" s="2"/>
+      <c r="E97" s="11"/>
+    </row>
+    <row r="98" spans="2:6">
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
-      <c r="D98" s="13"/>
-    </row>
-    <row r="99" spans="2:5">
+      <c r="D98" s="2"/>
+      <c r="E98" s="11"/>
+    </row>
+    <row r="99" spans="2:6">
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
-      <c r="D99" s="13"/>
-    </row>
-    <row r="100" spans="2:5">
+      <c r="D99" s="2"/>
+      <c r="E99" s="11"/>
+    </row>
+    <row r="100" spans="2:6">
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="13"/>
-    </row>
-    <row r="101" spans="2:5">
+      <c r="D100" s="2"/>
+      <c r="E100" s="11"/>
+    </row>
+    <row r="101" spans="2:6">
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
-      <c r="D101" s="13"/>
-    </row>
-    <row r="102" spans="2:5">
+      <c r="D101" s="2"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="1"/>
+    </row>
+    <row r="102" spans="2:6">
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
-      <c r="D102" s="13"/>
-      <c r="E102" s="1"/>
-    </row>
-    <row r="103" spans="2:5">
+      <c r="D102" s="2"/>
+      <c r="E102" s="11"/>
+    </row>
+    <row r="103" spans="2:6">
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
-      <c r="D103" s="13"/>
-    </row>
-    <row r="104" spans="2:5">
+      <c r="D103" s="2"/>
+      <c r="E103" s="11"/>
+    </row>
+    <row r="104" spans="2:6">
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
-      <c r="D104" s="13"/>
-    </row>
-    <row r="105" spans="2:5">
+      <c r="D104" s="2"/>
+      <c r="E104" s="11"/>
+    </row>
+    <row r="105" spans="2:6">
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
-      <c r="D105" s="13"/>
-    </row>
-    <row r="106" spans="2:5">
+      <c r="D105" s="2"/>
+      <c r="E105" s="11"/>
+    </row>
+    <row r="106" spans="2:6">
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
-      <c r="D106" s="13"/>
-    </row>
-    <row r="107" spans="2:5">
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="2:6">
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="2:5">
+      <c r="D107" s="2"/>
+      <c r="E107" s="11"/>
+    </row>
+    <row r="108" spans="2:6">
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
-      <c r="D108" s="13"/>
-    </row>
-    <row r="109" spans="2:5">
+      <c r="D108" s="2"/>
+      <c r="E108" s="11"/>
+    </row>
+    <row r="109" spans="2:6">
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
-      <c r="D109" s="13"/>
-    </row>
-    <row r="110" spans="2:5">
+      <c r="D109" s="2"/>
+      <c r="E109" s="11"/>
+    </row>
+    <row r="110" spans="2:6">
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
-      <c r="D110" s="13"/>
-    </row>
-    <row r="111" spans="2:5">
+      <c r="D110" s="2"/>
+      <c r="E110" s="11"/>
+    </row>
+    <row r="111" spans="2:6">
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
-      <c r="D111" s="13"/>
-    </row>
-    <row r="112" spans="2:5">
+      <c r="D111" s="2"/>
+      <c r="E111" s="11"/>
+    </row>
+    <row r="112" spans="2:6">
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
-      <c r="D112" s="13"/>
-    </row>
-    <row r="113" spans="2:7">
+      <c r="D112" s="2"/>
+      <c r="E112" s="11"/>
+    </row>
+    <row r="113" spans="2:8">
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
-      <c r="D113" s="13"/>
-    </row>
-    <row r="114" spans="2:7">
+      <c r="D113" s="2"/>
+      <c r="E113" s="11"/>
+    </row>
+    <row r="114" spans="2:8">
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
-      <c r="D114" s="13"/>
-    </row>
-    <row r="115" spans="2:7">
+      <c r="D114" s="2"/>
+      <c r="E114" s="11"/>
+    </row>
+    <row r="115" spans="2:8">
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
-      <c r="D115" s="13"/>
-    </row>
-    <row r="116" spans="2:7">
+      <c r="D115" s="2"/>
+      <c r="E115" s="11"/>
+      <c r="H115" s="2"/>
+    </row>
+    <row r="116" spans="2:8">
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
-      <c r="D116" s="13"/>
-      <c r="G116" s="2"/>
-    </row>
-    <row r="117" spans="2:7">
+      <c r="D116" s="2"/>
+      <c r="E116" s="11"/>
+      <c r="H116" s="2"/>
+    </row>
+    <row r="117" spans="2:8">
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
-      <c r="D117" s="13"/>
-      <c r="G117" s="2"/>
-    </row>
-    <row r="118" spans="2:7">
+      <c r="D117" s="2"/>
+      <c r="E117" s="11"/>
+      <c r="H117" s="2"/>
+    </row>
+    <row r="118" spans="2:8">
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
-      <c r="D118" s="13"/>
-      <c r="G118" s="2"/>
-    </row>
-    <row r="119" spans="2:7">
+      <c r="D118" s="2"/>
+      <c r="E118" s="11"/>
+    </row>
+    <row r="119" spans="2:8">
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
-      <c r="D119" s="13"/>
-    </row>
-    <row r="120" spans="2:7">
+      <c r="D119" s="2"/>
+      <c r="E119" s="11"/>
+    </row>
+    <row r="120" spans="2:8">
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
-      <c r="D120" s="13"/>
-    </row>
-    <row r="121" spans="2:7">
+      <c r="D120" s="2"/>
+      <c r="E120" s="11"/>
+    </row>
+    <row r="121" spans="2:8">
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
-      <c r="D121" s="13"/>
-    </row>
-    <row r="122" spans="2:7">
+      <c r="D121" s="2"/>
+      <c r="E121" s="11"/>
+    </row>
+    <row r="122" spans="2:8">
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
-      <c r="D122" s="13"/>
-    </row>
-    <row r="123" spans="2:7">
+      <c r="D122" s="2"/>
+      <c r="E122" s="11"/>
+    </row>
+    <row r="123" spans="2:8">
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
-      <c r="D123" s="13"/>
-    </row>
-    <row r="124" spans="2:7">
+      <c r="D123" s="2"/>
+      <c r="E123" s="11"/>
+    </row>
+    <row r="124" spans="2:8">
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
-      <c r="D124" s="13"/>
-    </row>
-    <row r="125" spans="2:7">
+      <c r="D124" s="2"/>
+      <c r="E124" s="11"/>
+    </row>
+    <row r="125" spans="2:8">
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
-      <c r="D125" s="13"/>
-    </row>
-    <row r="126" spans="2:7">
+      <c r="D125" s="2"/>
+      <c r="E125" s="11"/>
+    </row>
+    <row r="126" spans="2:8">
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
-      <c r="D126" s="13"/>
-    </row>
-    <row r="127" spans="2:7">
+      <c r="D126" s="2"/>
+      <c r="E126" s="11"/>
+    </row>
+    <row r="127" spans="2:8">
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
-      <c r="D127" s="13"/>
-    </row>
-    <row r="128" spans="2:7">
+      <c r="D127" s="2"/>
+      <c r="E127" s="11"/>
+    </row>
+    <row r="128" spans="2:8">
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
-      <c r="D128" s="13"/>
-    </row>
-    <row r="129" spans="2:4">
+      <c r="D128" s="2"/>
+      <c r="E128" s="11"/>
+    </row>
+    <row r="129" spans="2:5">
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
-      <c r="D129" s="13"/>
-    </row>
-    <row r="130" spans="2:4">
+      <c r="D129" s="2"/>
+      <c r="E129" s="11"/>
+    </row>
+    <row r="130" spans="2:5">
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
-      <c r="D130" s="13"/>
-    </row>
-    <row r="131" spans="2:4">
+      <c r="D130" s="2"/>
+      <c r="E130" s="11"/>
+    </row>
+    <row r="131" spans="2:5">
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
-      <c r="D131" s="13"/>
-    </row>
-    <row r="132" spans="2:4">
+      <c r="D131" s="2"/>
+      <c r="E131" s="11"/>
+    </row>
+    <row r="132" spans="2:5">
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
-      <c r="D132" s="13"/>
-    </row>
-    <row r="133" spans="2:4">
+      <c r="D132" s="2"/>
+      <c r="E132" s="11"/>
+    </row>
+    <row r="133" spans="2:5">
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
-      <c r="D133" s="13"/>
-    </row>
-    <row r="134" spans="2:4">
+      <c r="D133" s="2"/>
+      <c r="E133" s="11"/>
+    </row>
+    <row r="134" spans="2:5">
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
-      <c r="D134" s="13"/>
-    </row>
-    <row r="135" spans="2:4">
+      <c r="D134" s="2"/>
+      <c r="E134" s="11"/>
+    </row>
+    <row r="135" spans="2:5">
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
-      <c r="D135" s="13"/>
-    </row>
-    <row r="136" spans="2:4">
+      <c r="D135" s="2"/>
+      <c r="E135" s="11"/>
+    </row>
+    <row r="136" spans="2:5">
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
-      <c r="D136" s="13"/>
-    </row>
-    <row r="137" spans="2:4">
+      <c r="D136" s="2"/>
+      <c r="E136" s="11"/>
+    </row>
+    <row r="137" spans="2:5">
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
-      <c r="D137" s="13"/>
-    </row>
-    <row r="138" spans="2:4">
+      <c r="D137" s="2"/>
+      <c r="E137" s="11"/>
+    </row>
+    <row r="138" spans="2:5">
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
-      <c r="D138" s="13"/>
-    </row>
-    <row r="139" spans="2:4">
+      <c r="D138" s="2"/>
+      <c r="E138" s="11"/>
+    </row>
+    <row r="139" spans="2:5">
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
-      <c r="D139" s="13"/>
-    </row>
-    <row r="140" spans="2:4">
+      <c r="D139" s="2"/>
+      <c r="E139" s="11"/>
+    </row>
+    <row r="140" spans="2:5">
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
-      <c r="D140" s="13"/>
-    </row>
-    <row r="141" spans="2:4">
+      <c r="D140" s="2"/>
+      <c r="E140" s="11"/>
+    </row>
+    <row r="141" spans="2:5">
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
-      <c r="D141" s="13"/>
-    </row>
-    <row r="142" spans="2:4">
+      <c r="D141" s="2"/>
+      <c r="E141" s="11"/>
+    </row>
+    <row r="142" spans="2:5">
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
-      <c r="D142" s="13"/>
-    </row>
-    <row r="143" spans="2:4">
+      <c r="D142" s="2"/>
+      <c r="E142" s="11"/>
+    </row>
+    <row r="143" spans="2:5">
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
-      <c r="D143" s="13"/>
-    </row>
-    <row r="144" spans="2:4">
+      <c r="D143" s="2"/>
+      <c r="E143" s="11"/>
+    </row>
+    <row r="144" spans="2:5">
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
-      <c r="D144" s="13"/>
-    </row>
-    <row r="145" spans="2:4">
+      <c r="D144" s="2"/>
+      <c r="E144" s="11"/>
+    </row>
+    <row r="145" spans="2:5">
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
-      <c r="D145" s="13"/>
-    </row>
-    <row r="146" spans="2:4">
+      <c r="D145" s="2"/>
+      <c r="E145" s="11"/>
+    </row>
+    <row r="146" spans="2:5">
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
-      <c r="D146" s="13"/>
-    </row>
-    <row r="147" spans="2:4">
+      <c r="D146" s="2"/>
+      <c r="E146" s="11"/>
+    </row>
+    <row r="147" spans="2:5">
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
-      <c r="D147" s="13"/>
-    </row>
-    <row r="148" spans="2:4">
+      <c r="D147" s="2"/>
+      <c r="E147" s="11"/>
+    </row>
+    <row r="148" spans="2:5">
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
-      <c r="D148" s="13"/>
-    </row>
-    <row r="149" spans="2:4">
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="13"/>
-    </row>
-    <row r="167" spans="7:7">
-      <c r="G167" s="1"/>
-    </row>
-    <row r="168" spans="7:7">
-      <c r="G168" s="1"/>
-    </row>
-    <row r="169" spans="7:7">
-      <c r="G169" s="1"/>
-    </row>
-    <row r="170" spans="7:7">
-      <c r="G170" s="1"/>
-    </row>
-    <row r="171" spans="7:7">
-      <c r="G171" s="1"/>
-    </row>
-    <row r="172" spans="7:7">
-      <c r="G172" s="1"/>
-    </row>
-    <row r="225" spans="2:4">
+      <c r="D148" s="2"/>
+      <c r="E148" s="11"/>
+    </row>
+    <row r="166" spans="8:8">
+      <c r="H166" s="1"/>
+    </row>
+    <row r="167" spans="8:8">
+      <c r="H167" s="1"/>
+    </row>
+    <row r="168" spans="8:8">
+      <c r="H168" s="1"/>
+    </row>
+    <row r="169" spans="8:8">
+      <c r="H169" s="1"/>
+    </row>
+    <row r="170" spans="8:8">
+      <c r="H170" s="1"/>
+    </row>
+    <row r="171" spans="8:8">
+      <c r="H171" s="1"/>
+    </row>
+    <row r="224" spans="2:5">
+      <c r="B224" s="2"/>
+      <c r="C224" s="2"/>
+      <c r="D224" s="2"/>
+      <c r="E224" s="11"/>
+    </row>
+    <row r="225" spans="2:5">
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
-      <c r="D225" s="13"/>
-    </row>
-    <row r="226" spans="2:4">
+      <c r="D225" s="2"/>
+      <c r="E225" s="11"/>
+    </row>
+    <row r="226" spans="2:5">
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
-      <c r="D226" s="13"/>
-    </row>
-    <row r="227" spans="2:4">
+      <c r="D226" s="2"/>
+      <c r="E226" s="11"/>
+    </row>
+    <row r="227" spans="2:5">
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
-      <c r="D227" s="13"/>
-    </row>
-    <row r="228" spans="2:4">
+      <c r="D227" s="2"/>
+      <c r="E227" s="11"/>
+    </row>
+    <row r="228" spans="2:5">
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
-      <c r="D228" s="13"/>
-    </row>
-    <row r="229" spans="2:4">
+      <c r="D228" s="2"/>
+      <c r="E228" s="11"/>
+    </row>
+    <row r="229" spans="2:5">
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
-      <c r="D229" s="13"/>
-    </row>
-    <row r="230" spans="2:4">
+      <c r="D229" s="2"/>
+      <c r="E229" s="11"/>
+    </row>
+    <row r="230" spans="2:5">
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
-      <c r="D230" s="13"/>
-    </row>
-    <row r="231" spans="2:4">
+      <c r="D230" s="2"/>
+      <c r="E230" s="11"/>
+    </row>
+    <row r="231" spans="2:5">
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
-      <c r="D231" s="13"/>
-    </row>
-    <row r="232" spans="2:4">
+      <c r="D231" s="2"/>
+      <c r="E231" s="11"/>
+    </row>
+    <row r="232" spans="2:5">
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
-      <c r="D232" s="13"/>
-    </row>
-    <row r="233" spans="2:4">
+      <c r="D232" s="2"/>
+      <c r="E232" s="11"/>
+    </row>
+    <row r="233" spans="2:5">
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
-      <c r="D233" s="13"/>
-    </row>
-    <row r="234" spans="2:4">
+      <c r="D233" s="2"/>
+      <c r="E233" s="11"/>
+    </row>
+    <row r="234" spans="2:5">
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
-      <c r="D234" s="13"/>
-    </row>
-    <row r="235" spans="2:4">
+      <c r="D234" s="2"/>
+      <c r="E234" s="11"/>
+    </row>
+    <row r="235" spans="2:5">
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
-      <c r="D235" s="13"/>
-    </row>
-    <row r="236" spans="2:4">
+      <c r="D235" s="2"/>
+      <c r="E235" s="11"/>
+    </row>
+    <row r="236" spans="2:5">
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
-      <c r="D236" s="13"/>
-    </row>
-    <row r="237" spans="2:4">
+      <c r="D236" s="2"/>
+      <c r="E236" s="11"/>
+    </row>
+    <row r="237" spans="2:5">
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
-      <c r="D237" s="13"/>
-    </row>
-    <row r="238" spans="2:4">
+      <c r="D237" s="2"/>
+      <c r="E237" s="11"/>
+    </row>
+    <row r="238" spans="2:5">
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
-      <c r="D238" s="13"/>
-    </row>
-    <row r="239" spans="2:4">
+      <c r="D238" s="2"/>
+      <c r="E238" s="11"/>
+    </row>
+    <row r="239" spans="2:5">
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
-      <c r="D239" s="13"/>
-    </row>
-    <row r="240" spans="2:4">
+      <c r="D239" s="2"/>
+      <c r="E239" s="11"/>
+    </row>
+    <row r="240" spans="2:5">
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
-      <c r="D240" s="13"/>
-    </row>
-    <row r="241" spans="2:4">
+      <c r="D240" s="2"/>
+      <c r="E240" s="11"/>
+    </row>
+    <row r="241" spans="2:5">
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
-      <c r="D241" s="13"/>
-    </row>
-    <row r="242" spans="2:4">
+      <c r="D241" s="2"/>
+      <c r="E241" s="11"/>
+    </row>
+    <row r="242" spans="2:5">
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
-      <c r="D242" s="13"/>
-    </row>
-    <row r="243" spans="2:4">
+      <c r="D242" s="2"/>
+      <c r="E242" s="11"/>
+    </row>
+    <row r="243" spans="2:5">
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
-      <c r="D243" s="13"/>
-    </row>
-    <row r="244" spans="2:4">
+      <c r="D243" s="2"/>
+      <c r="E243" s="11"/>
+    </row>
+    <row r="244" spans="2:5">
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
-      <c r="D244" s="13"/>
-    </row>
-    <row r="245" spans="2:4">
+      <c r="D244" s="2"/>
+      <c r="E244" s="11"/>
+    </row>
+    <row r="245" spans="2:5">
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
-      <c r="D245" s="13"/>
-    </row>
-    <row r="246" spans="2:4">
+      <c r="D245" s="2"/>
+      <c r="E245" s="11"/>
+    </row>
+    <row r="246" spans="2:5">
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
-      <c r="D246" s="13"/>
-    </row>
-    <row r="247" spans="2:4">
+      <c r="D246" s="2"/>
+      <c r="E246" s="11"/>
+    </row>
+    <row r="247" spans="2:5">
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
-      <c r="D247" s="13"/>
-    </row>
-    <row r="248" spans="2:4">
+      <c r="D247" s="2"/>
+      <c r="E247" s="11"/>
+    </row>
+    <row r="248" spans="2:5">
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
-      <c r="D248" s="13"/>
-    </row>
-    <row r="249" spans="2:4">
+      <c r="D248" s="2"/>
+    </row>
+    <row r="249" spans="2:5">
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
-    </row>
-    <row r="250" spans="2:4">
+      <c r="D249" s="2"/>
+      <c r="E249" s="11"/>
+    </row>
+    <row r="250" spans="2:5">
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
-      <c r="D250" s="13"/>
-    </row>
-    <row r="251" spans="2:4">
+      <c r="D250" s="2"/>
+      <c r="E250" s="11"/>
+    </row>
+    <row r="251" spans="2:5">
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
-      <c r="D251" s="13"/>
-    </row>
-    <row r="252" spans="2:4">
+      <c r="D251" s="2"/>
+      <c r="E251" s="11"/>
+    </row>
+    <row r="252" spans="2:5">
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
-      <c r="D252" s="13"/>
-    </row>
-    <row r="253" spans="2:4">
+      <c r="D252" s="2"/>
+      <c r="E252" s="11"/>
+    </row>
+    <row r="253" spans="2:5">
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
-      <c r="D253" s="13"/>
-    </row>
-    <row r="254" spans="2:4">
+      <c r="D253" s="2"/>
+      <c r="E253" s="11"/>
+    </row>
+    <row r="254" spans="2:5">
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
-      <c r="D254" s="13"/>
-    </row>
-    <row r="255" spans="2:4">
+      <c r="D254" s="2"/>
+      <c r="E254" s="11"/>
+    </row>
+    <row r="255" spans="2:5">
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
-      <c r="D255" s="13"/>
-    </row>
-    <row r="256" spans="2:4">
-      <c r="B256" s="2"/>
-      <c r="C256" s="2"/>
-      <c r="D256" s="13"/>
-    </row>
-    <row r="939" spans="5:5">
-      <c r="E939" s="2"/>
-    </row>
-    <row r="1075" spans="2:3">
+      <c r="D255" s="2"/>
+      <c r="E255" s="11"/>
+    </row>
+    <row r="938" spans="6:6">
+      <c r="F938" s="2"/>
+    </row>
+    <row r="1074" spans="2:4">
+      <c r="B1074" s="2"/>
+      <c r="C1074" s="2"/>
+      <c r="D1074" s="2"/>
+    </row>
+    <row r="1075" spans="2:4">
       <c r="B1075" s="2"/>
       <c r="C1075" s="2"/>
-    </row>
-    <row r="1076" spans="2:3">
-      <c r="B1076" s="2"/>
-      <c r="C1076" s="2"/>
-    </row>
-    <row r="1201" spans="2:3">
+      <c r="D1075" s="2"/>
+    </row>
+    <row r="1200" spans="2:4">
+      <c r="B1200" s="2"/>
+      <c r="C1200" s="2"/>
+      <c r="D1200" s="2"/>
+    </row>
+    <row r="1201" spans="2:4">
       <c r="B1201" s="2"/>
       <c r="C1201" s="2"/>
-    </row>
-    <row r="1202" spans="2:3">
+      <c r="D1201" s="2"/>
+    </row>
+    <row r="1202" spans="2:4">
       <c r="B1202" s="2"/>
       <c r="C1202" s="2"/>
-    </row>
-    <row r="1203" spans="2:3">
+      <c r="D1202" s="2"/>
+    </row>
+    <row r="1203" spans="2:4">
       <c r="B1203" s="2"/>
       <c r="C1203" s="2"/>
-    </row>
-    <row r="1204" spans="2:3">
+      <c r="D1203" s="2"/>
+    </row>
+    <row r="1204" spans="2:4">
       <c r="B1204" s="2"/>
       <c r="C1204" s="2"/>
-    </row>
-    <row r="1205" spans="2:3">
+      <c r="D1204" s="2"/>
+    </row>
+    <row r="1205" spans="2:4">
       <c r="B1205" s="2"/>
       <c r="C1205" s="2"/>
-    </row>
-    <row r="1206" spans="2:3">
-      <c r="B1206" s="2"/>
-      <c r="C1206" s="2"/>
-    </row>
-    <row r="1251" spans="2:6">
-      <c r="E1251" s="2"/>
+      <c r="D1205" s="2"/>
+    </row>
+    <row r="1250" spans="2:7">
+      <c r="F1250" s="2"/>
+      <c r="G1250" s="2"/>
+    </row>
+    <row r="1251" spans="2:7">
       <c r="F1251" s="2"/>
-    </row>
-    <row r="1252" spans="2:6">
-      <c r="E1252" s="2"/>
+      <c r="G1251" s="2"/>
+    </row>
+    <row r="1252" spans="2:7">
       <c r="F1252" s="2"/>
-    </row>
-    <row r="1253" spans="2:6">
-      <c r="E1253" s="2"/>
-      <c r="F1253" s="2"/>
-    </row>
-    <row r="1255" spans="2:6">
+      <c r="G1252" s="2"/>
+    </row>
+    <row r="1254" spans="2:7">
+      <c r="B1254" s="2"/>
+      <c r="C1254" s="2"/>
+      <c r="D1254" s="2"/>
+    </row>
+    <row r="1255" spans="2:7">
       <c r="B1255" s="2"/>
       <c r="C1255" s="2"/>
-    </row>
-    <row r="1256" spans="2:6">
+      <c r="D1255" s="2"/>
+    </row>
+    <row r="1256" spans="2:7">
       <c r="B1256" s="2"/>
       <c r="C1256" s="2"/>
-    </row>
-    <row r="1257" spans="2:6">
+      <c r="D1256" s="2"/>
+    </row>
+    <row r="1257" spans="2:7">
       <c r="B1257" s="2"/>
       <c r="C1257" s="2"/>
-    </row>
-    <row r="1258" spans="2:6">
+      <c r="D1257" s="2"/>
+    </row>
+    <row r="1258" spans="2:7">
       <c r="B1258" s="2"/>
       <c r="C1258" s="2"/>
-    </row>
-    <row r="1259" spans="2:6">
-      <c r="B1259" s="2"/>
-      <c r="C1259" s="2"/>
-    </row>
-    <row r="1278" spans="2:3">
+      <c r="D1258" s="2"/>
+    </row>
+    <row r="1277" spans="2:4">
+      <c r="B1277" s="2"/>
+      <c r="C1277" s="2"/>
+      <c r="D1277" s="2"/>
+    </row>
+    <row r="1278" spans="2:4">
       <c r="B1278" s="2"/>
       <c r="C1278" s="2"/>
-    </row>
-    <row r="1279" spans="2:3">
+      <c r="D1278" s="2"/>
+    </row>
+    <row r="1279" spans="2:4">
       <c r="B1279" s="2"/>
       <c r="C1279" s="2"/>
-    </row>
-    <row r="1280" spans="2:3">
+      <c r="D1279" s="2"/>
+    </row>
+    <row r="1280" spans="2:4">
       <c r="B1280" s="2"/>
       <c r="C1280" s="2"/>
-    </row>
-    <row r="1281" spans="2:3">
+      <c r="D1280" s="2"/>
+    </row>
+    <row r="1281" spans="2:4">
       <c r="B1281" s="2"/>
       <c r="C1281" s="2"/>
-    </row>
-    <row r="1282" spans="2:3">
+      <c r="D1281" s="2"/>
+    </row>
+    <row r="1282" spans="2:4">
       <c r="B1282" s="2"/>
       <c r="C1282" s="2"/>
-    </row>
-    <row r="1283" spans="2:3">
+      <c r="D1282" s="2"/>
+    </row>
+    <row r="1283" spans="2:4">
       <c r="B1283" s="2"/>
       <c r="C1283" s="2"/>
-    </row>
-    <row r="1284" spans="2:3">
-      <c r="B1284" s="2"/>
-      <c r="C1284" s="2"/>
-    </row>
-    <row r="1286" spans="2:3">
+      <c r="D1283" s="2"/>
+    </row>
+    <row r="1285" spans="2:4">
+      <c r="B1285" s="2"/>
+      <c r="C1285" s="2"/>
+      <c r="D1285" s="2"/>
+    </row>
+    <row r="1286" spans="2:4">
       <c r="B1286" s="2"/>
       <c r="C1286" s="2"/>
-    </row>
-    <row r="1287" spans="2:3">
+      <c r="D1286" s="2"/>
+    </row>
+    <row r="1287" spans="2:4">
       <c r="B1287" s="2"/>
       <c r="C1287" s="2"/>
-    </row>
-    <row r="1288" spans="2:3">
+      <c r="D1287" s="2"/>
+    </row>
+    <row r="1288" spans="2:4">
       <c r="B1288" s="2"/>
       <c r="C1288" s="2"/>
-    </row>
-    <row r="1289" spans="2:3">
+      <c r="D1288" s="2"/>
+    </row>
+    <row r="1289" spans="2:4">
       <c r="B1289" s="2"/>
       <c r="C1289" s="2"/>
-    </row>
-    <row r="1290" spans="2:3">
+      <c r="D1289" s="2"/>
+    </row>
+    <row r="1290" spans="2:4">
       <c r="B1290" s="2"/>
       <c r="C1290" s="2"/>
-    </row>
-    <row r="1291" spans="2:3">
-      <c r="B1291" s="2"/>
-      <c r="C1291" s="2"/>
-    </row>
-    <row r="1343" spans="2:3">
+      <c r="D1290" s="2"/>
+    </row>
+    <row r="1342" spans="2:4">
+      <c r="B1342" s="2"/>
+      <c r="C1342" s="2"/>
+      <c r="D1342" s="2"/>
+    </row>
+    <row r="1343" spans="2:4">
       <c r="B1343" s="2"/>
       <c r="C1343" s="2"/>
-    </row>
-    <row r="1344" spans="2:3">
+      <c r="D1343" s="2"/>
+    </row>
+    <row r="1344" spans="2:4">
       <c r="B1344" s="2"/>
       <c r="C1344" s="2"/>
-    </row>
-    <row r="1345" spans="2:3">
+      <c r="D1344" s="2"/>
+    </row>
+    <row r="1345" spans="2:4">
       <c r="B1345" s="2"/>
       <c r="C1345" s="2"/>
-    </row>
-    <row r="1346" spans="2:3">
-      <c r="B1346" s="2"/>
-      <c r="C1346" s="2"/>
-    </row>
-    <row r="1348" spans="2:3">
+      <c r="D1345" s="2"/>
+    </row>
+    <row r="1347" spans="2:4">
+      <c r="B1347" s="2"/>
+      <c r="C1347" s="2"/>
+      <c r="D1347" s="2"/>
+    </row>
+    <row r="1348" spans="2:4">
       <c r="B1348" s="2"/>
       <c r="C1348" s="2"/>
-    </row>
-    <row r="1349" spans="2:3">
+      <c r="D1348" s="2"/>
+    </row>
+    <row r="1349" spans="2:4">
       <c r="B1349" s="2"/>
       <c r="C1349" s="2"/>
-    </row>
-    <row r="1350" spans="2:3">
+      <c r="D1349" s="2"/>
+    </row>
+    <row r="1350" spans="2:4">
       <c r="B1350" s="2"/>
       <c r="C1350" s="2"/>
-    </row>
-    <row r="1351" spans="2:3">
-      <c r="B1351" s="2"/>
-      <c r="C1351" s="2"/>
-    </row>
-    <row r="1386" spans="2:3">
+      <c r="D1350" s="2"/>
+    </row>
+    <row r="1385" spans="2:4">
+      <c r="B1385" s="2"/>
+      <c r="C1385" s="2"/>
+      <c r="D1385" s="2"/>
+    </row>
+    <row r="1386" spans="2:4">
       <c r="B1386" s="2"/>
       <c r="C1386" s="2"/>
-    </row>
-    <row r="1387" spans="2:3">
+      <c r="D1386" s="2"/>
+    </row>
+    <row r="1387" spans="2:4">
       <c r="B1387" s="2"/>
       <c r="C1387" s="2"/>
-    </row>
-    <row r="1388" spans="2:3">
+      <c r="D1387" s="2"/>
+    </row>
+    <row r="1388" spans="2:4">
       <c r="B1388" s="2"/>
       <c r="C1388" s="2"/>
-    </row>
-    <row r="1389" spans="2:3">
+      <c r="D1388" s="2"/>
+    </row>
+    <row r="1389" spans="2:4">
       <c r="B1389" s="2"/>
       <c r="C1389" s="2"/>
-    </row>
-    <row r="1390" spans="2:3">
+      <c r="D1389" s="2"/>
+    </row>
+    <row r="1390" spans="2:4">
       <c r="B1390" s="2"/>
       <c r="C1390" s="2"/>
-    </row>
-    <row r="1391" spans="2:3">
-      <c r="B1391" s="2"/>
-      <c r="C1391" s="2"/>
-    </row>
-    <row r="1433" spans="4:6">
-      <c r="E1433" s="2"/>
+      <c r="D1390" s="2"/>
+    </row>
+    <row r="1432" spans="5:7">
+      <c r="F1432" s="2"/>
+      <c r="G1432" s="2"/>
+    </row>
+    <row r="1433" spans="5:7">
+      <c r="E1433" s="12"/>
       <c r="F1433" s="2"/>
-    </row>
-    <row r="1434" spans="4:6">
-      <c r="D1434" s="14"/>
-      <c r="E1434" s="2"/>
+      <c r="G1433" s="2"/>
+    </row>
+    <row r="1434" spans="5:7">
+      <c r="E1434" s="12"/>
       <c r="F1434" s="2"/>
-    </row>
-    <row r="1435" spans="4:6">
-      <c r="D1435" s="14"/>
-      <c r="E1435" s="2"/>
+      <c r="G1434" s="2"/>
+    </row>
+    <row r="1435" spans="5:7">
+      <c r="E1435" s="12"/>
       <c r="F1435" s="2"/>
-    </row>
-    <row r="1436" spans="4:6">
-      <c r="D1436" s="14"/>
-      <c r="E1436" s="2"/>
+      <c r="G1435" s="2"/>
+    </row>
+    <row r="1436" spans="5:7">
       <c r="F1436" s="2"/>
-    </row>
-    <row r="1437" spans="4:6">
-      <c r="E1437" s="2"/>
-      <c r="F1437" s="2"/>
-    </row>
-    <row r="1500" spans="2:3">
+      <c r="G1436" s="2"/>
+    </row>
+    <row r="1499" spans="2:4">
+      <c r="B1499" s="2"/>
+      <c r="C1499" s="2"/>
+      <c r="D1499" s="2"/>
+    </row>
+    <row r="1500" spans="2:4">
       <c r="B1500" s="2"/>
       <c r="C1500" s="2"/>
-    </row>
-    <row r="1501" spans="2:3">
+      <c r="D1500" s="2"/>
+    </row>
+    <row r="1501" spans="2:4">
       <c r="B1501" s="2"/>
       <c r="C1501" s="2"/>
-    </row>
-    <row r="1502" spans="2:3">
+      <c r="D1501" s="2"/>
+    </row>
+    <row r="1502" spans="2:4">
       <c r="B1502" s="2"/>
       <c r="C1502" s="2"/>
-    </row>
-    <row r="1503" spans="2:3">
-      <c r="B1503" s="2"/>
-      <c r="C1503" s="2"/>
+      <c r="D1502" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="A2:H45">
+    <sortCondition ref="H2:H45"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>